<commit_message>
Fix probe attributes to match answers
</commit_message>
<xml_diff>
--- a/Stim_AssociateMasterList.xlsx
+++ b/Stim_AssociateMasterList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\Elyse_FHWordOA\experiment_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52C517AA-53B4-4963-BDF9-7795FDFF70E9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B9358F4-4B26-4A8D-AA66-BBE6AC2C1908}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{35527C65-4FF7-AE4E-91DC-C83F90262CB4}"/>
   </bookViews>
@@ -72,9 +72,6 @@
     <t>Male</t>
   </si>
   <si>
-    <t>Old</t>
-  </si>
-  <si>
     <t>White</t>
   </si>
   <si>
@@ -87,21 +84,12 @@
     <t>RADIO</t>
   </si>
   <si>
-    <t xml:space="preserve">Young </t>
-  </si>
-  <si>
-    <t>Non White</t>
-  </si>
-  <si>
     <t>Stim/Face/TMWmale23neutral.jpg</t>
   </si>
   <si>
     <t>ROAD</t>
   </si>
   <si>
-    <t>Young</t>
-  </si>
-  <si>
     <t>Stim/Face/TSFBfemale65-2neutral.jpg</t>
   </si>
   <si>
@@ -807,9 +795,6 @@
     <t>Stim/House/hstim44.bmp</t>
   </si>
   <si>
-    <t>GOLD</t>
-  </si>
-  <si>
     <t>Stim/House/hstim103.bmp</t>
   </si>
   <si>
@@ -835,6 +820,21 @@
   </si>
   <si>
     <t>UID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Younger </t>
+  </si>
+  <si>
+    <t>Younger</t>
+  </si>
+  <si>
+    <t>Older</t>
+  </si>
+  <si>
+    <t>GOlder</t>
+  </si>
+  <si>
+    <t>Not White</t>
   </si>
 </sst>
 </file>
@@ -1234,7 +1234,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1278,17 +1278,17 @@
         <v>11</v>
       </c>
       <c r="F2" t="s">
+        <v>264</v>
+      </c>
+      <c r="G2" t="s">
         <v>12</v>
       </c>
-      <c r="G2" t="s">
-        <v>13</v>
-      </c>
       <c r="H2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I2">
         <f t="shared" ref="I2:I33" ca="1" si="0" xml:space="preserve"> RAND()</f>
-        <v>0.1871175475507042</v>
+        <v>0.68356255724639103</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -1296,10 +1296,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>15</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>16</v>
       </c>
       <c r="D3" t="s">
         <v>10</v>
@@ -1308,17 +1308,17 @@
         <v>11</v>
       </c>
       <c r="F3" t="s">
-        <v>17</v>
+        <v>262</v>
       </c>
       <c r="G3" t="s">
-        <v>18</v>
+        <v>266</v>
       </c>
       <c r="H3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.84855315376634799</v>
+        <v>0.338201116760944</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -1326,10 +1326,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D4" t="s">
         <v>10</v>
@@ -1338,17 +1338,17 @@
         <v>11</v>
       </c>
       <c r="F4" t="s">
-        <v>21</v>
+        <v>263</v>
       </c>
       <c r="G4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.81712803877937545</v>
+        <v>0.41218370518132763</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -1356,29 +1356,29 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D5" t="s">
         <v>10</v>
       </c>
       <c r="E5" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F5" t="s">
-        <v>12</v>
+        <v>264</v>
       </c>
       <c r="G5" t="s">
-        <v>18</v>
+        <v>266</v>
       </c>
       <c r="H5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.9522778223288727</v>
+        <v>0.65007752365009019</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -1386,29 +1386,29 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D6" t="s">
         <v>10</v>
       </c>
       <c r="E6" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F6" t="s">
+        <v>264</v>
+      </c>
+      <c r="G6" t="s">
         <v>12</v>
       </c>
-      <c r="G6" t="s">
-        <v>13</v>
-      </c>
       <c r="H6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I6">
         <f t="shared" ca="1" si="0"/>
-        <v>0.21465642950543062</v>
+        <v>0.80392274096881988</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -1416,29 +1416,29 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D7" t="s">
         <v>10</v>
       </c>
       <c r="E7" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F7" t="s">
-        <v>21</v>
+        <v>263</v>
       </c>
       <c r="G7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I7">
         <f t="shared" ca="1" si="0"/>
-        <v>0.59893034849590887</v>
+        <v>0.41391857567898094</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -1446,10 +1446,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D8" t="s">
         <v>10</v>
@@ -1458,17 +1458,17 @@
         <v>11</v>
       </c>
       <c r="F8" t="s">
-        <v>17</v>
+        <v>262</v>
       </c>
       <c r="G8" t="s">
-        <v>18</v>
+        <v>266</v>
       </c>
       <c r="H8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I8">
         <f t="shared" ca="1" si="0"/>
-        <v>0.62229765214968102</v>
+        <v>5.1740088879483448E-2</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -1476,10 +1476,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D9" t="s">
         <v>10</v>
@@ -1488,17 +1488,17 @@
         <v>11</v>
       </c>
       <c r="F9" t="s">
+        <v>264</v>
+      </c>
+      <c r="G9" t="s">
         <v>12</v>
       </c>
-      <c r="G9" t="s">
-        <v>13</v>
-      </c>
       <c r="H9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I9">
         <f t="shared" ca="1" si="0"/>
-        <v>0.59395076875464481</v>
+        <v>0.5369501741766457</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -1506,10 +1506,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D10" t="s">
         <v>10</v>
@@ -1518,17 +1518,17 @@
         <v>11</v>
       </c>
       <c r="F10" t="s">
+        <v>264</v>
+      </c>
+      <c r="G10" t="s">
         <v>12</v>
       </c>
-      <c r="G10" t="s">
-        <v>13</v>
-      </c>
       <c r="H10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I10">
         <f t="shared" ca="1" si="0"/>
-        <v>0.7332855276726461</v>
+        <v>0.7120101890444881</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -1536,10 +1536,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D11" t="s">
         <v>10</v>
@@ -1548,17 +1548,17 @@
         <v>11</v>
       </c>
       <c r="F11" t="s">
+        <v>264</v>
+      </c>
+      <c r="G11" t="s">
         <v>12</v>
       </c>
-      <c r="G11" t="s">
-        <v>13</v>
-      </c>
       <c r="H11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I11">
         <f t="shared" ca="1" si="0"/>
-        <v>3.8453283474641609E-2</v>
+        <v>0.60216802293493177</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -1566,29 +1566,29 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D12" t="s">
         <v>10</v>
       </c>
       <c r="E12" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F12" t="s">
-        <v>21</v>
+        <v>263</v>
       </c>
       <c r="G12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I12">
         <f t="shared" ca="1" si="0"/>
-        <v>0.6303142734316376</v>
+        <v>0.98137025919966114</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -1596,29 +1596,29 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D13" t="s">
         <v>10</v>
       </c>
       <c r="E13" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F13" t="s">
-        <v>12</v>
+        <v>264</v>
       </c>
       <c r="G13" t="s">
-        <v>18</v>
+        <v>266</v>
       </c>
       <c r="H13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I13">
         <f t="shared" ca="1" si="0"/>
-        <v>0.5404330273521698</v>
+        <v>2.9219908610370826E-2</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -1626,10 +1626,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D14" t="s">
         <v>10</v>
@@ -1638,17 +1638,17 @@
         <v>11</v>
       </c>
       <c r="F14" t="s">
-        <v>17</v>
+        <v>262</v>
       </c>
       <c r="G14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I14">
         <f t="shared" ca="1" si="0"/>
-        <v>0.47523569579280966</v>
+        <v>0.71050070293663825</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -1656,29 +1656,29 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D15" t="s">
         <v>10</v>
       </c>
       <c r="E15" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F15" t="s">
+        <v>264</v>
+      </c>
+      <c r="G15" t="s">
         <v>12</v>
       </c>
-      <c r="G15" t="s">
-        <v>13</v>
-      </c>
       <c r="H15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I15">
         <f t="shared" ca="1" si="0"/>
-        <v>5.1593384341259707E-3</v>
+        <v>0.36780517499762533</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -1686,29 +1686,29 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D16" t="s">
         <v>10</v>
       </c>
       <c r="E16" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F16" t="s">
-        <v>17</v>
+        <v>262</v>
       </c>
       <c r="G16" t="s">
-        <v>18</v>
+        <v>266</v>
       </c>
       <c r="H16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I16">
         <f t="shared" ca="1" si="0"/>
-        <v>0.89392590439153052</v>
+        <v>0.77199093606904001</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -1716,10 +1716,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D17" t="s">
         <v>10</v>
@@ -1728,17 +1728,17 @@
         <v>11</v>
       </c>
       <c r="F17" t="s">
+        <v>264</v>
+      </c>
+      <c r="G17" t="s">
         <v>12</v>
       </c>
-      <c r="G17" t="s">
-        <v>13</v>
-      </c>
       <c r="H17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I17">
         <f t="shared" ca="1" si="0"/>
-        <v>0.18016864431545798</v>
+        <v>0.37090660573079981</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -1746,29 +1746,29 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D18" t="s">
         <v>10</v>
       </c>
       <c r="E18" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F18" t="s">
-        <v>17</v>
+        <v>262</v>
       </c>
       <c r="G18" t="s">
-        <v>18</v>
+        <v>266</v>
       </c>
       <c r="H18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I18">
         <f t="shared" ca="1" si="0"/>
-        <v>0.66509488054720844</v>
+        <v>0.58892490744326065</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -1776,29 +1776,29 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D19" t="s">
         <v>10</v>
       </c>
       <c r="E19" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F19" t="s">
-        <v>21</v>
+        <v>263</v>
       </c>
       <c r="G19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I19">
         <f t="shared" ca="1" si="0"/>
-        <v>0.5853268999977147</v>
+        <v>0.19189935058834784</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -1806,10 +1806,10 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D20" t="s">
         <v>10</v>
@@ -1818,17 +1818,17 @@
         <v>11</v>
       </c>
       <c r="F20" t="s">
+        <v>264</v>
+      </c>
+      <c r="G20" t="s">
         <v>12</v>
       </c>
-      <c r="G20" t="s">
-        <v>13</v>
-      </c>
       <c r="H20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I20">
         <f t="shared" ca="1" si="0"/>
-        <v>0.94406501293479417</v>
+        <v>0.88371922360032262</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -1836,10 +1836,10 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D21" t="s">
         <v>10</v>
@@ -1848,17 +1848,17 @@
         <v>11</v>
       </c>
       <c r="F21" t="s">
-        <v>21</v>
+        <v>263</v>
       </c>
       <c r="G21" t="s">
-        <v>18</v>
+        <v>266</v>
       </c>
       <c r="H21" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I21">
         <f t="shared" ca="1" si="0"/>
-        <v>0.837696286417554</v>
+        <v>0.89510018276536274</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -1866,10 +1866,10 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D22" t="s">
         <v>10</v>
@@ -1878,17 +1878,17 @@
         <v>11</v>
       </c>
       <c r="F22" t="s">
-        <v>12</v>
+        <v>264</v>
       </c>
       <c r="G22" t="s">
-        <v>18</v>
+        <v>266</v>
       </c>
       <c r="H22" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I22">
         <f t="shared" ca="1" si="0"/>
-        <v>0.33615039264640234</v>
+        <v>0.21109293585150912</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -1896,10 +1896,10 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D23" t="s">
         <v>10</v>
@@ -1908,17 +1908,17 @@
         <v>11</v>
       </c>
       <c r="F23" t="s">
-        <v>17</v>
+        <v>262</v>
       </c>
       <c r="G23" t="s">
-        <v>18</v>
+        <v>266</v>
       </c>
       <c r="H23" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I23">
         <f t="shared" ca="1" si="0"/>
-        <v>0.55909159101855144</v>
+        <v>0.29889157725117599</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -1926,29 +1926,29 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D24" t="s">
         <v>10</v>
       </c>
       <c r="E24" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F24" t="s">
+        <v>264</v>
+      </c>
+      <c r="G24" t="s">
         <v>12</v>
       </c>
-      <c r="G24" t="s">
-        <v>13</v>
-      </c>
       <c r="H24" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I24">
         <f t="shared" ca="1" si="0"/>
-        <v>0.42949594272692238</v>
+        <v>0.70247960311627899</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -1956,29 +1956,29 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D25" t="s">
         <v>10</v>
       </c>
       <c r="E25" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F25" t="s">
-        <v>21</v>
+        <v>263</v>
       </c>
       <c r="G25" t="s">
-        <v>18</v>
+        <v>266</v>
       </c>
       <c r="H25" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I25">
         <f t="shared" ca="1" si="0"/>
-        <v>0.6938958561223042</v>
+        <v>0.59089216601012451</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -1986,10 +1986,10 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D26" t="s">
         <v>10</v>
@@ -1998,17 +1998,17 @@
         <v>11</v>
       </c>
       <c r="F26" t="s">
-        <v>21</v>
+        <v>263</v>
       </c>
       <c r="G26" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H26" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I26">
         <f t="shared" ca="1" si="0"/>
-        <v>0.54897022106776883</v>
+        <v>0.65416259486174677</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -2016,10 +2016,10 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D27" t="s">
         <v>10</v>
@@ -2028,17 +2028,17 @@
         <v>11</v>
       </c>
       <c r="F27" t="s">
-        <v>21</v>
+        <v>263</v>
       </c>
       <c r="G27" t="s">
-        <v>18</v>
+        <v>266</v>
       </c>
       <c r="H27" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I27">
         <f t="shared" ca="1" si="0"/>
-        <v>0.94406971149431451</v>
+        <v>0.4863114484411053</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -2046,10 +2046,10 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D28" t="s">
         <v>10</v>
@@ -2058,17 +2058,17 @@
         <v>11</v>
       </c>
       <c r="F28" t="s">
-        <v>12</v>
+        <v>264</v>
       </c>
       <c r="G28" t="s">
-        <v>18</v>
+        <v>266</v>
       </c>
       <c r="H28" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I28">
         <f t="shared" ca="1" si="0"/>
-        <v>0.92386673009833908</v>
+        <v>0.8461424206315592</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -2076,10 +2076,10 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D29" t="s">
         <v>10</v>
@@ -2088,17 +2088,17 @@
         <v>11</v>
       </c>
       <c r="F29" t="s">
-        <v>21</v>
+        <v>263</v>
       </c>
       <c r="G29" t="s">
-        <v>18</v>
+        <v>266</v>
       </c>
       <c r="H29" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I29">
         <f t="shared" ca="1" si="0"/>
-        <v>0.14929192568462679</v>
+        <v>0.31730448099786102</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -2106,10 +2106,10 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D30" t="s">
         <v>10</v>
@@ -2118,17 +2118,17 @@
         <v>11</v>
       </c>
       <c r="F30" t="s">
-        <v>21</v>
+        <v>263</v>
       </c>
       <c r="G30" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H30" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I30">
         <f t="shared" ca="1" si="0"/>
-        <v>6.9410333309495864E-2</v>
+        <v>0.38741546450556075</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -2136,10 +2136,10 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D31" t="s">
         <v>10</v>
@@ -2148,17 +2148,17 @@
         <v>11</v>
       </c>
       <c r="F31" t="s">
-        <v>21</v>
+        <v>263</v>
       </c>
       <c r="G31" t="s">
-        <v>18</v>
+        <v>266</v>
       </c>
       <c r="H31" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I31">
         <f t="shared" ca="1" si="0"/>
-        <v>1.9860612735230543E-2</v>
+        <v>0.64461758765718469</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
@@ -2166,29 +2166,29 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D32" t="s">
         <v>10</v>
       </c>
       <c r="E32" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F32" t="s">
-        <v>17</v>
+        <v>262</v>
       </c>
       <c r="G32" t="s">
-        <v>18</v>
+        <v>266</v>
       </c>
       <c r="H32" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I32">
         <f t="shared" ca="1" si="0"/>
-        <v>0.64479832673894311</v>
+        <v>0.61461352531525604</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
@@ -2196,10 +2196,10 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D33" t="s">
         <v>10</v>
@@ -2208,17 +2208,17 @@
         <v>11</v>
       </c>
       <c r="F33" t="s">
-        <v>21</v>
+        <v>263</v>
       </c>
       <c r="G33" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H33" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I33">
         <f t="shared" ca="1" si="0"/>
-        <v>0.97398000554591335</v>
+        <v>0.23639353170616906</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
@@ -2226,29 +2226,29 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D34" t="s">
         <v>10</v>
       </c>
       <c r="E34" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F34" t="s">
-        <v>17</v>
+        <v>262</v>
       </c>
       <c r="G34" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H34" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I34">
         <f t="shared" ref="I34:I65" ca="1" si="1" xml:space="preserve"> RAND()</f>
-        <v>0.75589362959157158</v>
+        <v>0.65011765939849198</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
@@ -2256,10 +2256,10 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D35" t="s">
         <v>10</v>
@@ -2268,17 +2268,17 @@
         <v>11</v>
       </c>
       <c r="F35" t="s">
-        <v>21</v>
+        <v>263</v>
       </c>
       <c r="G35" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H35" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I35">
         <f t="shared" ca="1" si="1"/>
-        <v>0.82777448640268636</v>
+        <v>0.17560331013254438</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
@@ -2286,10 +2286,10 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D36" t="s">
         <v>10</v>
@@ -2298,17 +2298,17 @@
         <v>11</v>
       </c>
       <c r="F36" t="s">
-        <v>21</v>
+        <v>263</v>
       </c>
       <c r="G36" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H36" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I36">
         <f t="shared" ca="1" si="1"/>
-        <v>0.33580983164177913</v>
+        <v>0.3830754617945723</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
@@ -2316,29 +2316,29 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D37" t="s">
         <v>10</v>
       </c>
       <c r="E37" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F37" t="s">
+        <v>264</v>
+      </c>
+      <c r="G37" t="s">
         <v>12</v>
       </c>
-      <c r="G37" t="s">
-        <v>13</v>
-      </c>
       <c r="H37" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I37">
         <f t="shared" ca="1" si="1"/>
-        <v>0.39877169033980475</v>
+        <v>8.3148613427662665E-3</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
@@ -2346,10 +2346,10 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D38" t="s">
         <v>10</v>
@@ -2358,17 +2358,17 @@
         <v>11</v>
       </c>
       <c r="F38" t="s">
-        <v>21</v>
+        <v>263</v>
       </c>
       <c r="G38" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H38" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I38">
         <f t="shared" ca="1" si="1"/>
-        <v>0.50575470624754892</v>
+        <v>0.98543934720366855</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
@@ -2376,29 +2376,29 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D39" t="s">
         <v>10</v>
       </c>
       <c r="E39" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F39" t="s">
-        <v>21</v>
+        <v>263</v>
       </c>
       <c r="G39" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H39" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I39">
         <f t="shared" ca="1" si="1"/>
-        <v>0.95754885048983907</v>
+        <v>0.66676216223144391</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
@@ -2406,29 +2406,29 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D40" t="s">
         <v>10</v>
       </c>
       <c r="E40" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F40" t="s">
-        <v>21</v>
+        <v>263</v>
       </c>
       <c r="G40" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H40" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I40">
         <f t="shared" ca="1" si="1"/>
-        <v>0.38616337940597556</v>
+        <v>0.16025535053393425</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
@@ -2436,29 +2436,29 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D41" t="s">
         <v>10</v>
       </c>
       <c r="E41" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F41" t="s">
-        <v>21</v>
+        <v>263</v>
       </c>
       <c r="G41" t="s">
-        <v>18</v>
+        <v>266</v>
       </c>
       <c r="H41" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I41">
         <f t="shared" ca="1" si="1"/>
-        <v>0.28332079277041211</v>
+        <v>0.54560678018582376</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
@@ -2466,10 +2466,10 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D42" t="s">
         <v>10</v>
@@ -2478,17 +2478,17 @@
         <v>11</v>
       </c>
       <c r="F42" t="s">
+        <v>264</v>
+      </c>
+      <c r="G42" t="s">
         <v>12</v>
       </c>
-      <c r="G42" t="s">
-        <v>13</v>
-      </c>
       <c r="H42" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I42">
         <f t="shared" ca="1" si="1"/>
-        <v>0.64078011318135519</v>
+        <v>0.15530614867100001</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
@@ -2496,29 +2496,29 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D43" t="s">
         <v>10</v>
       </c>
       <c r="E43" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F43" t="s">
-        <v>21</v>
+        <v>263</v>
       </c>
       <c r="G43" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H43" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I43">
         <f t="shared" ca="1" si="1"/>
-        <v>0.53426687378261428</v>
+        <v>0.45815935195396451</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
@@ -2526,10 +2526,10 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D44" t="s">
         <v>10</v>
@@ -2538,17 +2538,17 @@
         <v>11</v>
       </c>
       <c r="F44" t="s">
+        <v>264</v>
+      </c>
+      <c r="G44" t="s">
         <v>12</v>
       </c>
-      <c r="G44" t="s">
-        <v>13</v>
-      </c>
       <c r="H44" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I44">
         <f t="shared" ca="1" si="1"/>
-        <v>0.92594347223231521</v>
+        <v>0.34491931631927797</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
@@ -2556,29 +2556,29 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="D45" t="s">
         <v>10</v>
       </c>
       <c r="E45" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F45" t="s">
+        <v>264</v>
+      </c>
+      <c r="G45" t="s">
         <v>12</v>
       </c>
-      <c r="G45" t="s">
-        <v>13</v>
-      </c>
       <c r="H45" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I45">
         <f t="shared" ca="1" si="1"/>
-        <v>0.14335328966375349</v>
+        <v>0.695766062779545</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
@@ -2586,29 +2586,29 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D46" t="s">
         <v>10</v>
       </c>
       <c r="E46" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F46" t="s">
+        <v>264</v>
+      </c>
+      <c r="G46" t="s">
         <v>12</v>
       </c>
-      <c r="G46" t="s">
-        <v>13</v>
-      </c>
       <c r="H46" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I46">
         <f t="shared" ca="1" si="1"/>
-        <v>0.53709006027409911</v>
+        <v>0.82161197845521439</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
@@ -2616,10 +2616,10 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D47" t="s">
         <v>10</v>
@@ -2628,17 +2628,17 @@
         <v>11</v>
       </c>
       <c r="F47" t="s">
-        <v>12</v>
+        <v>264</v>
       </c>
       <c r="G47" t="s">
-        <v>18</v>
+        <v>266</v>
       </c>
       <c r="H47" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I47">
         <f t="shared" ca="1" si="1"/>
-        <v>0.47252626475305837</v>
+        <v>0.63974731045205901</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
@@ -2646,29 +2646,29 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D48" t="s">
         <v>10</v>
       </c>
       <c r="E48" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F48" t="s">
-        <v>21</v>
+        <v>263</v>
       </c>
       <c r="G48" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H48" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I48">
         <f t="shared" ca="1" si="1"/>
-        <v>0.43469995376254067</v>
+        <v>0.23142286054999994</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
@@ -2676,10 +2676,10 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D49" t="s">
         <v>10</v>
@@ -2688,17 +2688,17 @@
         <v>11</v>
       </c>
       <c r="F49" t="s">
-        <v>21</v>
+        <v>263</v>
       </c>
       <c r="G49" t="s">
-        <v>18</v>
+        <v>266</v>
       </c>
       <c r="H49" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I49">
         <f t="shared" ca="1" si="1"/>
-        <v>0.73622368155277651</v>
+        <v>0.72540473433679376</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
@@ -2706,29 +2706,29 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D50" t="s">
         <v>10</v>
       </c>
       <c r="E50" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F50" t="s">
-        <v>21</v>
+        <v>263</v>
       </c>
       <c r="G50" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H50" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I50">
         <f t="shared" ca="1" si="1"/>
-        <v>8.6226627693938629E-2</v>
+        <v>7.7677658788747883E-2</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
@@ -2736,29 +2736,29 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="D51" t="s">
         <v>10</v>
       </c>
       <c r="E51" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F51" t="s">
+        <v>264</v>
+      </c>
+      <c r="G51" t="s">
         <v>12</v>
       </c>
-      <c r="G51" t="s">
-        <v>13</v>
-      </c>
       <c r="H51" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I51">
         <f t="shared" ca="1" si="1"/>
-        <v>0.98085589565279163</v>
+        <v>0.90757354690473857</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
@@ -2766,10 +2766,10 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="D52" t="s">
         <v>10</v>
@@ -2778,17 +2778,17 @@
         <v>11</v>
       </c>
       <c r="F52" t="s">
+        <v>264</v>
+      </c>
+      <c r="G52" t="s">
         <v>12</v>
       </c>
-      <c r="G52" t="s">
-        <v>13</v>
-      </c>
       <c r="H52" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I52">
         <f t="shared" ca="1" si="1"/>
-        <v>0.48349399664837367</v>
+        <v>0.97453735988471168</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
@@ -2796,29 +2796,29 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D53" t="s">
         <v>10</v>
       </c>
       <c r="E53" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F53" t="s">
+        <v>264</v>
+      </c>
+      <c r="G53" t="s">
         <v>12</v>
       </c>
-      <c r="G53" t="s">
-        <v>13</v>
-      </c>
       <c r="H53" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I53">
         <f t="shared" ca="1" si="1"/>
-        <v>5.7776121235666444E-3</v>
+        <v>0.32756613435728232</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
@@ -2826,29 +2826,29 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="D54" t="s">
         <v>10</v>
       </c>
       <c r="E54" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F54" t="s">
-        <v>17</v>
+        <v>262</v>
       </c>
       <c r="G54" t="s">
-        <v>18</v>
+        <v>266</v>
       </c>
       <c r="H54" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I54">
         <f t="shared" ca="1" si="1"/>
-        <v>0.78792364969964157</v>
+        <v>0.98084556081038687</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
@@ -2856,29 +2856,29 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="D55" t="s">
         <v>10</v>
       </c>
       <c r="E55" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F55" t="s">
-        <v>21</v>
+        <v>263</v>
       </c>
       <c r="G55" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H55" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I55">
         <f t="shared" ca="1" si="1"/>
-        <v>0.70572734000766724</v>
+        <v>0.10356057351842074</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
@@ -2886,29 +2886,29 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="D56" t="s">
         <v>10</v>
       </c>
       <c r="E56" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F56" t="s">
-        <v>17</v>
+        <v>262</v>
       </c>
       <c r="G56" t="s">
-        <v>18</v>
+        <v>266</v>
       </c>
       <c r="H56" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I56">
         <f t="shared" ca="1" si="1"/>
-        <v>0.64066648172044272</v>
+        <v>0.83525256391846492</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
@@ -2916,29 +2916,29 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="D57" t="s">
         <v>10</v>
       </c>
       <c r="E57" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F57" t="s">
+        <v>264</v>
+      </c>
+      <c r="G57" t="s">
         <v>12</v>
       </c>
-      <c r="G57" t="s">
-        <v>13</v>
-      </c>
       <c r="H57" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I57">
         <f t="shared" ca="1" si="1"/>
-        <v>0.47504064111228395</v>
+        <v>0.3042097826976915</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
@@ -2946,29 +2946,29 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="D58" t="s">
         <v>10</v>
       </c>
       <c r="E58" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F58" t="s">
-        <v>12</v>
+        <v>264</v>
       </c>
       <c r="G58" t="s">
-        <v>18</v>
+        <v>266</v>
       </c>
       <c r="H58" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I58">
         <f t="shared" ca="1" si="1"/>
-        <v>0.33273114889825672</v>
+        <v>0.71146842384175757</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
@@ -2976,10 +2976,10 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D59" t="s">
         <v>10</v>
@@ -2988,17 +2988,17 @@
         <v>11</v>
       </c>
       <c r="F59" t="s">
-        <v>21</v>
+        <v>263</v>
       </c>
       <c r="G59" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H59" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I59">
         <f t="shared" ca="1" si="1"/>
-        <v>0.72723920203946368</v>
+        <v>0.34405946820116473</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
@@ -3006,29 +3006,29 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="D60" t="s">
         <v>10</v>
       </c>
       <c r="E60" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F60" t="s">
-        <v>21</v>
+        <v>263</v>
       </c>
       <c r="G60" t="s">
-        <v>18</v>
+        <v>266</v>
       </c>
       <c r="H60" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I60">
         <f t="shared" ca="1" si="1"/>
-        <v>0.25080334733687437</v>
+        <v>0.33733464285058412</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
@@ -3036,10 +3036,10 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D61" t="s">
         <v>10</v>
@@ -3048,17 +3048,17 @@
         <v>11</v>
       </c>
       <c r="F61" t="s">
-        <v>21</v>
+        <v>263</v>
       </c>
       <c r="G61" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H61" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I61">
         <f t="shared" ca="1" si="1"/>
-        <v>0.71090627798412587</v>
+        <v>0.8930175393046198</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
@@ -3066,29 +3066,29 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
+        <v>133</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="D62" t="s">
+        <v>135</v>
+      </c>
+      <c r="E62" t="s">
+        <v>136</v>
+      </c>
+      <c r="F62" t="s">
         <v>137</v>
       </c>
-      <c r="C62" s="3" t="s">
+      <c r="G62" t="s">
         <v>138</v>
       </c>
-      <c r="D62" t="s">
-        <v>139</v>
-      </c>
-      <c r="E62" t="s">
-        <v>140</v>
-      </c>
-      <c r="F62" t="s">
-        <v>141</v>
-      </c>
-      <c r="G62" t="s">
-        <v>142</v>
-      </c>
       <c r="H62" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="I62">
         <f t="shared" ca="1" si="1"/>
-        <v>0.32551505670390701</v>
+        <v>0.99547297851119121</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
@@ -3096,29 +3096,29 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D63" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E63" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="F63" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="G63" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="H63" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="I63">
         <f t="shared" ca="1" si="1"/>
-        <v>0.16485731206954979</v>
+        <v>4.2766712289386E-3</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
@@ -3126,29 +3126,29 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D64" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E64" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="F64" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="G64" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="H64" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="I64">
         <f t="shared" ca="1" si="1"/>
-        <v>0.95925665921183756</v>
+        <v>0.40664726342779356</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
@@ -3156,29 +3156,29 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="D65" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E65" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="F65" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="G65" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="H65" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="I65">
         <f t="shared" ca="1" si="1"/>
-        <v>0.67942299823266195</v>
+        <v>0.6321930521452378</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
@@ -3186,29 +3186,29 @@
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="D66" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E66" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="F66" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="G66" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="H66" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="I66">
         <f t="shared" ref="I66:I97" ca="1" si="2" xml:space="preserve"> RAND()</f>
-        <v>0.88989637476130068</v>
+        <v>0.3957014874043332</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
@@ -3216,29 +3216,29 @@
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="D67" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E67" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="F67" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="G67" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="H67" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="I67">
         <f t="shared" ca="1" si="2"/>
-        <v>0.41847576786832419</v>
+        <v>0.64253350985592117</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
@@ -3246,29 +3246,29 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="D68" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E68" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="F68" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="G68" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="H68" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="I68">
         <f t="shared" ca="1" si="2"/>
-        <v>0.85274309101607904</v>
+        <v>0.10763338136412437</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
@@ -3276,29 +3276,29 @@
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="D69" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E69" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="F69" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="G69" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="H69" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="I69">
         <f t="shared" ca="1" si="2"/>
-        <v>0.94417594105633285</v>
+        <v>0.48467424347390053</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
@@ -3306,29 +3306,29 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="D70" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E70" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="F70" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="G70" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="H70" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="I70">
         <f t="shared" ca="1" si="2"/>
-        <v>0.88478395839963464</v>
+        <v>0.32468634997592705</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
@@ -3336,29 +3336,29 @@
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="D71" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E71" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="F71" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="G71" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="H71" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="I71">
         <f t="shared" ca="1" si="2"/>
-        <v>0.31649163268207814</v>
+        <v>0.42439422650429892</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
@@ -3366,29 +3366,29 @@
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="D72" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E72" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="F72" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="G72" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="H72" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="I72">
         <f t="shared" ca="1" si="2"/>
-        <v>0.30007387920092465</v>
+        <v>0.13349798169056981</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
@@ -3396,29 +3396,29 @@
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="D73" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E73" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="F73" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="G73" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="H73" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="I73">
         <f t="shared" ca="1" si="2"/>
-        <v>0.51257328393159896</v>
+        <v>0.98712665414293588</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
@@ -3426,29 +3426,29 @@
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="D74" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E74" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="F74" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="G74" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="H74" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="I74">
         <f t="shared" ca="1" si="2"/>
-        <v>1.6927790841752E-2</v>
+        <v>0.72676009044609913</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
@@ -3456,29 +3456,29 @@
         <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D75" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E75" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="F75" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="G75" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="H75" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="I75">
         <f t="shared" ca="1" si="2"/>
-        <v>0.52509947581139049</v>
+        <v>0.86850162764925221</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
@@ -3486,29 +3486,29 @@
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="D76" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E76" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="F76" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="G76" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="H76" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="I76">
         <f t="shared" ca="1" si="2"/>
-        <v>0.24539572895686912</v>
+        <v>0.32967647112243648</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
@@ -3516,29 +3516,29 @@
         <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D77" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E77" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="F77" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="G77" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="H77" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="I77">
         <f t="shared" ca="1" si="2"/>
-        <v>0.10284964816133013</v>
+        <v>0.96756654196834824</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
@@ -3546,29 +3546,29 @@
         <v>77</v>
       </c>
       <c r="B78" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="D78" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E78" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="F78" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="G78" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="H78" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="I78">
         <f t="shared" ca="1" si="2"/>
-        <v>0.8382340268549705</v>
+        <v>0.53435393009557397</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
@@ -3576,29 +3576,29 @@
         <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="D79" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E79" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="F79" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="G79" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="H79" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="I79">
         <f t="shared" ca="1" si="2"/>
-        <v>0.65920687963925417</v>
+        <v>0.26190159626858167</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
@@ -3606,29 +3606,29 @@
         <v>79</v>
       </c>
       <c r="B80" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="D80" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E80" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="F80" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="G80" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="H80" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="I80">
         <f t="shared" ca="1" si="2"/>
-        <v>0.88174882652726871</v>
+        <v>0.28375193072171256</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
@@ -3636,29 +3636,29 @@
         <v>80</v>
       </c>
       <c r="B81" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="D81" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E81" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="F81" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="G81" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="H81" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="I81">
         <f t="shared" ca="1" si="2"/>
-        <v>0.60837081183297259</v>
+        <v>0.45728149089026204</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
@@ -3666,29 +3666,29 @@
         <v>81</v>
       </c>
       <c r="B82" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="D82" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E82" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="F82" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="G82" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="H82" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="I82">
         <f t="shared" ca="1" si="2"/>
-        <v>9.8957491075313153E-2</v>
+        <v>0.72592565393425401</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
@@ -3696,29 +3696,29 @@
         <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="D83" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E83" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="F83" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="G83" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="H83" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="I83">
         <f t="shared" ca="1" si="2"/>
-        <v>0.75684111541828902</v>
+        <v>0.66404633897782972</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
@@ -3726,29 +3726,29 @@
         <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="D84" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E84" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="F84" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="G84" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="H84" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="I84">
         <f t="shared" ca="1" si="2"/>
-        <v>0.47193690065081983</v>
+        <v>0.94202139971714471</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
@@ -3756,29 +3756,29 @@
         <v>84</v>
       </c>
       <c r="B85" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="D85" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E85" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="F85" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="G85" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="H85" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="I85">
         <f t="shared" ca="1" si="2"/>
-        <v>0.29327692467999378</v>
+        <v>0.35740710223899952</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">
@@ -3786,29 +3786,29 @@
         <v>85</v>
       </c>
       <c r="B86" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="D86" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E86" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="F86" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="G86" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="H86" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="I86">
         <f t="shared" ca="1" si="2"/>
-        <v>0.66823747119394672</v>
+        <v>0.89008056460937035</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
@@ -3816,29 +3816,29 @@
         <v>86</v>
       </c>
       <c r="B87" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="D87" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E87" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="F87" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="G87" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="H87" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="I87">
         <f t="shared" ca="1" si="2"/>
-        <v>0.13682158007381873</v>
+        <v>0.86194733568001947</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
@@ -3846,29 +3846,29 @@
         <v>87</v>
       </c>
       <c r="B88" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="D88" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E88" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="F88" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="G88" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="H88" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="I88">
         <f t="shared" ca="1" si="2"/>
-        <v>0.49291031303446708</v>
+        <v>0.94278634931662042</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
@@ -3876,29 +3876,29 @@
         <v>88</v>
       </c>
       <c r="B89" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="D89" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E89" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="F89" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="G89" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="H89" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="I89">
         <f t="shared" ca="1" si="2"/>
-        <v>0.96467830693909074</v>
+        <v>0.63545518545415225</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
@@ -3906,29 +3906,29 @@
         <v>89</v>
       </c>
       <c r="B90" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="D90" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E90" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="F90" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="G90" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="H90" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="I90">
         <f t="shared" ca="1" si="2"/>
-        <v>0.61777086672539783</v>
+        <v>0.59640126695972007</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">
@@ -3936,29 +3936,29 @@
         <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="D91" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E91" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="F91" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="G91" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="H91" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="I91">
         <f t="shared" ca="1" si="2"/>
-        <v>0.28214141537979842</v>
+        <v>0.48036534396041863</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.25">
@@ -3966,29 +3966,29 @@
         <v>91</v>
       </c>
       <c r="B92" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="D92" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E92" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="F92" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="G92" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="H92" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="I92">
         <f t="shared" ca="1" si="2"/>
-        <v>0.86747484448421275</v>
+        <v>0.89653683571343179</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.25">
@@ -3996,29 +3996,29 @@
         <v>92</v>
       </c>
       <c r="B93" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="D93" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E93" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="F93" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="G93" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="H93" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="I93">
         <f t="shared" ca="1" si="2"/>
-        <v>0.22346030124449934</v>
+        <v>0.95364399278242618</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.25">
@@ -4026,29 +4026,29 @@
         <v>93</v>
       </c>
       <c r="B94" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D94" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E94" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="F94" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="G94" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="H94" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="I94">
         <f t="shared" ca="1" si="2"/>
-        <v>0.57708772922715668</v>
+        <v>0.61055452663389165</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.25">
@@ -4056,29 +4056,29 @@
         <v>94</v>
       </c>
       <c r="B95" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="D95" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E95" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="F95" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="G95" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="H95" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="I95">
         <f t="shared" ca="1" si="2"/>
-        <v>0.39123148680343967</v>
+        <v>0.7346042272791945</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.25">
@@ -4086,29 +4086,29 @@
         <v>95</v>
       </c>
       <c r="B96" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="D96" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E96" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="F96" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="G96" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="H96" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="I96">
         <f t="shared" ca="1" si="2"/>
-        <v>0.59776233564785397</v>
+        <v>0.82136906587637215</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
@@ -4116,29 +4116,29 @@
         <v>96</v>
       </c>
       <c r="B97" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="D97" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E97" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="F97" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="G97" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="H97" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="I97">
         <f t="shared" ca="1" si="2"/>
-        <v>0.19229576958303241</v>
+        <v>0.89784676352879322</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
@@ -4146,29 +4146,29 @@
         <v>97</v>
       </c>
       <c r="B98" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="D98" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E98" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="F98" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="G98" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="H98" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="I98">
         <f t="shared" ref="I98:I121" ca="1" si="3" xml:space="preserve"> RAND()</f>
-        <v>0.54118589006864226</v>
+        <v>0.98665035602835405</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.25">
@@ -4176,29 +4176,29 @@
         <v>98</v>
       </c>
       <c r="B99" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="D99" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E99" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="F99" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="G99" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="H99" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="I99">
         <f t="shared" ca="1" si="3"/>
-        <v>0.54439070642629483</v>
+        <v>0.4912222928507407</v>
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
@@ -4206,29 +4206,29 @@
         <v>99</v>
       </c>
       <c r="B100" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="D100" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E100" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="F100" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="G100" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="H100" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="I100">
         <f t="shared" ca="1" si="3"/>
-        <v>0.11448466338899277</v>
+        <v>0.21826772458466948</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
@@ -4236,29 +4236,29 @@
         <v>100</v>
       </c>
       <c r="B101" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="D101" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E101" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="F101" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="G101" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="H101" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="I101">
         <f t="shared" ca="1" si="3"/>
-        <v>6.1509218973310964E-2</v>
+        <v>0.58320065584920389</v>
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.25">
@@ -4266,29 +4266,29 @@
         <v>101</v>
       </c>
       <c r="B102" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="C102" s="3" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="D102" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E102" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="F102" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="G102" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="H102" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="I102">
         <f t="shared" ca="1" si="3"/>
-        <v>0.48783128832967781</v>
+        <v>0.54153131904045593</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.25">
@@ -4296,29 +4296,29 @@
         <v>102</v>
       </c>
       <c r="B103" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="C103" s="3" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="D103" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E103" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="F103" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="G103" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="H103" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="I103">
         <f t="shared" ca="1" si="3"/>
-        <v>0.89592344280951453</v>
+        <v>0.33865296095183162</v>
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.25">
@@ -4326,29 +4326,29 @@
         <v>103</v>
       </c>
       <c r="B104" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="C104" s="3" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="D104" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E104" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="F104" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="G104" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="H104" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="I104">
         <f t="shared" ca="1" si="3"/>
-        <v>0.95962464117814361</v>
+        <v>6.8042747307959339E-2</v>
       </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.25">
@@ -4356,29 +4356,29 @@
         <v>104</v>
       </c>
       <c r="B105" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="C105" s="3" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="D105" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E105" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="F105" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="G105" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="H105" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="I105">
         <f t="shared" ca="1" si="3"/>
-        <v>0.62546193852117971</v>
+        <v>0.49332792132711345</v>
       </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.25">
@@ -4386,29 +4386,29 @@
         <v>105</v>
       </c>
       <c r="B106" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C106" s="3" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="D106" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E106" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="F106" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="G106" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="H106" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="I106">
         <f t="shared" ca="1" si="3"/>
-        <v>0.4798327345348955</v>
+        <v>0.25145297197093119</v>
       </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.25">
@@ -4416,29 +4416,29 @@
         <v>106</v>
       </c>
       <c r="B107" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="C107" s="3" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="D107" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E107" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="F107" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="G107" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="H107" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="I107">
         <f t="shared" ca="1" si="3"/>
-        <v>0.92909952158998288</v>
+        <v>0.74522264399540261</v>
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.25">
@@ -4446,29 +4446,29 @@
         <v>107</v>
       </c>
       <c r="B108" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="C108" s="3" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="D108" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E108" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="F108" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="G108" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="H108" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="I108">
         <f t="shared" ca="1" si="3"/>
-        <v>0.65747765604018193</v>
+        <v>0.71011938016493725</v>
       </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.25">
@@ -4476,29 +4476,29 @@
         <v>108</v>
       </c>
       <c r="B109" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="C109" s="3" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="D109" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E109" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="F109" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="G109" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="H109" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="I109">
         <f t="shared" ca="1" si="3"/>
-        <v>0.53854565512016961</v>
+        <v>0.57992849765238275</v>
       </c>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.25">
@@ -4506,29 +4506,29 @@
         <v>109</v>
       </c>
       <c r="B110" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="C110" s="3" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="D110" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E110" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="F110" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="G110" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="H110" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="I110">
         <f t="shared" ca="1" si="3"/>
-        <v>0.91958366422998816</v>
+        <v>0.37857242278124137</v>
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.25">
@@ -4536,29 +4536,29 @@
         <v>110</v>
       </c>
       <c r="B111" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="C111" s="3" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="D111" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E111" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="F111" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="G111" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="H111" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="I111">
         <f t="shared" ca="1" si="3"/>
-        <v>8.3035447521866423E-2</v>
+        <v>0.30420094394138875</v>
       </c>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.25">
@@ -4566,29 +4566,29 @@
         <v>111</v>
       </c>
       <c r="B112" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="C112" s="3" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="D112" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E112" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="F112" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="G112" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="H112" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="I112">
         <f t="shared" ca="1" si="3"/>
-        <v>0.85734000219439355</v>
+        <v>0.76152217675753753</v>
       </c>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.25">
@@ -4596,29 +4596,29 @@
         <v>112</v>
       </c>
       <c r="B113" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="C113" s="3" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="D113" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E113" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="F113" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="G113" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="H113" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="I113">
         <f t="shared" ca="1" si="3"/>
-        <v>0.84120602484119844</v>
+        <v>0.99643961128405956</v>
       </c>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.25">
@@ -4626,29 +4626,29 @@
         <v>113</v>
       </c>
       <c r="B114" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="C114" s="3" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="D114" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E114" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="F114" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="G114" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="H114" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="I114">
         <f t="shared" ca="1" si="3"/>
-        <v>0.5005163423229797</v>
+        <v>0.8657227181512116</v>
       </c>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.25">
@@ -4656,29 +4656,29 @@
         <v>114</v>
       </c>
       <c r="B115" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="C115" s="3" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="D115" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E115" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="F115" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="G115" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="H115" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="I115">
         <f t="shared" ca="1" si="3"/>
-        <v>0.72531955009711524</v>
+        <v>0.95837934146435011</v>
       </c>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.25">
@@ -4686,29 +4686,29 @@
         <v>115</v>
       </c>
       <c r="B116" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="C116" s="3" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="D116" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E116" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="F116" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="G116" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="H116" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="I116">
         <f t="shared" ca="1" si="3"/>
-        <v>0.515570704850006</v>
+        <v>0.92552043144061658</v>
       </c>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.25">
@@ -4716,29 +4716,29 @@
         <v>116</v>
       </c>
       <c r="B117" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="C117" s="3" t="s">
-        <v>257</v>
+        <v>265</v>
       </c>
       <c r="D117" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E117" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="F117" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="G117" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="H117" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="I117">
         <f t="shared" ca="1" si="3"/>
-        <v>0.40804047448401504</v>
+        <v>0.38916794172298208</v>
       </c>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.25">
@@ -4746,29 +4746,29 @@
         <v>117</v>
       </c>
       <c r="B118" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="C118" s="3" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="D118" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E118" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="F118" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="G118" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="H118" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="I118">
         <f t="shared" ca="1" si="3"/>
-        <v>0.6919931652630531</v>
+        <v>0.2153421263662687</v>
       </c>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.25">
@@ -4776,29 +4776,29 @@
         <v>118</v>
       </c>
       <c r="B119" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="C119" s="3" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="D119" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E119" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="F119" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="G119" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="H119" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="I119">
         <f t="shared" ca="1" si="3"/>
-        <v>0.19458689617753044</v>
+        <v>0.87377893464255685</v>
       </c>
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.25">
@@ -4806,29 +4806,29 @@
         <v>119</v>
       </c>
       <c r="B120" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="C120" s="3" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="D120" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E120" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="F120" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="G120" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="H120" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="I120">
         <f t="shared" ca="1" si="3"/>
-        <v>0.52113345244751696</v>
+        <v>0.51618192734046187</v>
       </c>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.25">
@@ -4836,29 +4836,29 @@
         <v>120</v>
       </c>
       <c r="B121" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="C121" s="3" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="D121" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E121" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="F121" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="G121" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="H121" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="I121">
         <f t="shared" ca="1" si="3"/>
-        <v>0.38210992980534908</v>
+        <v>0.72694028400025912</v>
       </c>
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>